<commit_message>
create supervised learning files
</commit_message>
<xml_diff>
--- a/03. Planilhas/Catalogo variaveis v3.xlsx
+++ b/03. Planilhas/Catalogo variaveis v3.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="404">
   <si>
     <t>TIPOBITO</t>
   </si>
@@ -1117,9 +1117,6 @@
   </si>
   <si>
     <t>Formato aaaa-mm-dd</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Tirar causas</t>
@@ -1692,8 +1689,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:K224"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1746,7 +1743,7 @@
         <v>357</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1781,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -1816,7 +1813,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K5" s="17"/>
     </row>
@@ -1852,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K6" s="17"/>
     </row>
@@ -1888,10 +1885,10 @@
         <v>1</v>
       </c>
       <c r="J7" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>375</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="8" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1929,10 +1926,10 @@
         <v>359</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1965,10 +1962,10 @@
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="20" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="39.6" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
@@ -2003,7 +2000,7 @@
         <v>360</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2038,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K11" s="17"/>
     </row>
@@ -2077,7 +2074,7 @@
         <v>361</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -2112,10 +2109,10 @@
         <v>1</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -2150,13 +2147,13 @@
         <v>1</v>
       </c>
       <c r="J14" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="K14" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="K14" s="17" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -2189,7 +2186,7 @@
       </c>
       <c r="J15" s="17"/>
       <c r="K15" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="158.4" hidden="1" x14ac:dyDescent="0.25">
@@ -2224,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K16" s="17"/>
     </row>
@@ -2260,7 +2257,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K17" s="17"/>
     </row>
@@ -2436,7 +2433,7 @@
       </c>
       <c r="K22" s="17"/>
     </row>
-    <row r="23" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>41</v>
       </c>
@@ -2469,7 +2466,7 @@
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2508,7 +2505,7 @@
       </c>
       <c r="K24" s="17"/>
     </row>
-    <row r="25" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>45</v>
       </c>
@@ -2541,7 +2538,7 @@
       </c>
       <c r="J25" s="17"/>
       <c r="K25" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
@@ -2580,7 +2577,7 @@
       </c>
       <c r="K26" s="17"/>
     </row>
-    <row r="27" spans="2:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
@@ -2613,7 +2610,7 @@
       </c>
       <c r="J27" s="17"/>
       <c r="K27" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -2652,7 +2649,7 @@
       </c>
       <c r="K28" s="17"/>
     </row>
-    <row r="29" spans="2:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>53</v>
       </c>
@@ -2685,7 +2682,7 @@
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -2720,10 +2717,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="66" hidden="1" x14ac:dyDescent="0.25">
@@ -2758,10 +2755,10 @@
         <v>1</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
@@ -2800,7 +2797,7 @@
       </c>
       <c r="K32" s="17"/>
     </row>
-    <row r="33" spans="2:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>61</v>
       </c>
@@ -2833,7 +2830,7 @@
       </c>
       <c r="J33" s="17"/>
       <c r="K33" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="2:11" ht="66" hidden="1" x14ac:dyDescent="0.25">
@@ -2868,10 +2865,10 @@
         <v>1</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="35" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2976,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K37" s="17"/>
     </row>
@@ -3150,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K42" s="17"/>
     </row>
@@ -3222,7 +3219,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K44" s="17"/>
     </row>
@@ -3294,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K46" s="17"/>
     </row>
@@ -3366,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K48" s="17"/>
     </row>
@@ -3472,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K51" s="17"/>
     </row>
@@ -3544,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K53" s="17"/>
     </row>
@@ -3584,7 +3581,7 @@
       </c>
       <c r="K54" s="17"/>
     </row>
-    <row r="55" spans="2:11" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>105</v>
       </c>
@@ -3617,7 +3614,7 @@
       </c>
       <c r="J55" s="17"/>
       <c r="K55" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="56" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -3656,7 +3653,7 @@
       </c>
       <c r="K56" s="17"/>
     </row>
-    <row r="57" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>109</v>
       </c>
@@ -3689,7 +3686,7 @@
       </c>
       <c r="J57" s="17"/>
       <c r="K57" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -3728,7 +3725,7 @@
       </c>
       <c r="K58" s="17"/>
     </row>
-    <row r="59" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>113</v>
       </c>
@@ -3761,7 +3758,7 @@
       </c>
       <c r="J59" s="17"/>
       <c r="K59" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="60" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -3800,7 +3797,7 @@
       </c>
       <c r="K60" s="17"/>
     </row>
-    <row r="61" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>117</v>
       </c>
@@ -3833,10 +3830,10 @@
       </c>
       <c r="J61" s="17"/>
       <c r="K61" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>119</v>
       </c>
@@ -3868,7 +3865,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K62" s="17"/>
     </row>
@@ -3904,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K63" s="17"/>
     </row>
@@ -3940,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K64" s="17"/>
     </row>
@@ -4078,7 +4075,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K68" s="17"/>
     </row>
@@ -4114,7 +4111,7 @@
         <v>1</v>
       </c>
       <c r="J69" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K69" s="17"/>
     </row>
@@ -4150,7 +4147,7 @@
         <v>0</v>
       </c>
       <c r="J70" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K70" s="17"/>
     </row>
@@ -4186,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K71" s="17"/>
     </row>
@@ -4258,7 +4255,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K73" s="17"/>
     </row>
@@ -4328,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="J75" s="21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K75" s="17"/>
     </row>
@@ -4638,7 +4635,7 @@
       <c r="J84" s="21"/>
       <c r="K84" s="17"/>
     </row>
-    <row r="85" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
         <v>163</v>
       </c>
@@ -4773,7 +4770,7 @@
       </c>
       <c r="J88" s="21"/>
       <c r="K88" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="89" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -4878,7 +4875,7 @@
       <c r="J91" s="21"/>
       <c r="K91" s="17"/>
     </row>
-    <row r="92" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
         <v>177</v>
       </c>
@@ -4945,7 +4942,7 @@
       </c>
       <c r="J93" s="21"/>
       <c r="K93" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="94" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -4981,7 +4978,7 @@
       </c>
       <c r="J94" s="21"/>
       <c r="K94" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="95" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -5086,7 +5083,7 @@
       <c r="J97" s="21"/>
       <c r="K97" s="17"/>
     </row>
-    <row r="98" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
         <v>189</v>
       </c>
@@ -5187,7 +5184,7 @@
       </c>
       <c r="J100" s="21"/>
       <c r="K100" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="101" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -5258,7 +5255,7 @@
       <c r="J102" s="21"/>
       <c r="K102" s="17"/>
     </row>
-    <row r="103" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
         <v>200</v>
       </c>
@@ -5970,10 +5967,10 @@
         <v>0</v>
       </c>
       <c r="J123" s="17" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K123" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="124" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -6009,7 +6006,7 @@
       </c>
       <c r="J124" s="17"/>
       <c r="K124" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="125" spans="2:11" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
@@ -6044,7 +6041,7 @@
         <v>0</v>
       </c>
       <c r="J125" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K125" s="17"/>
     </row>
@@ -6080,11 +6077,11 @@
         <v>0</v>
       </c>
       <c r="J126" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K126" s="17"/>
     </row>
-    <row r="127" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
         <v>233</v>
       </c>
@@ -6116,13 +6113,13 @@
         <v>1</v>
       </c>
       <c r="J127" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K127" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="128" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="128" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
         <v>235</v>
       </c>
@@ -6154,13 +6151,13 @@
         <v>1</v>
       </c>
       <c r="J128" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K128" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="129" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="129" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
         <v>237</v>
       </c>
@@ -6192,13 +6189,13 @@
         <v>1</v>
       </c>
       <c r="J129" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K129" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="130" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="130" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
         <v>239</v>
       </c>
@@ -6230,10 +6227,10 @@
         <v>1</v>
       </c>
       <c r="J130" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K130" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="131" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -6268,7 +6265,7 @@
         <v>1</v>
       </c>
       <c r="J131" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K131" s="17"/>
     </row>
@@ -6304,7 +6301,7 @@
         <v>1</v>
       </c>
       <c r="J132" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K132" s="17"/>
     </row>
@@ -6340,7 +6337,7 @@
         <v>1</v>
       </c>
       <c r="J133" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K133" s="17"/>
     </row>
@@ -6376,7 +6373,7 @@
         <v>1</v>
       </c>
       <c r="J134" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K134" s="17"/>
     </row>
@@ -6412,7 +6409,7 @@
         <v>0</v>
       </c>
       <c r="J135" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K135" s="17"/>
     </row>
@@ -6516,7 +6513,7 @@
         <v>0</v>
       </c>
       <c r="J138" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K138" s="17"/>
     </row>
@@ -6552,11 +6549,11 @@
         <v>0</v>
       </c>
       <c r="J139" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K139" s="17"/>
     </row>
-    <row r="140" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
         <v>259</v>
       </c>
@@ -6588,13 +6585,13 @@
         <v>1</v>
       </c>
       <c r="J140" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K140" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="141" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="141" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
         <v>261</v>
       </c>
@@ -6626,13 +6623,13 @@
         <v>1</v>
       </c>
       <c r="J141" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K141" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="142" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="142" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
         <v>263</v>
       </c>
@@ -6664,13 +6661,13 @@
         <v>1</v>
       </c>
       <c r="J142" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K142" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="143" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="143" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
         <v>265</v>
       </c>
@@ -6702,10 +6699,10 @@
         <v>1</v>
       </c>
       <c r="J143" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K143" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="144" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -6740,7 +6737,7 @@
         <v>1</v>
       </c>
       <c r="J144" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K144" s="17"/>
     </row>
@@ -6776,7 +6773,7 @@
         <v>1</v>
       </c>
       <c r="J145" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K145" s="17"/>
     </row>
@@ -6812,7 +6809,7 @@
         <v>1</v>
       </c>
       <c r="J146" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K146" s="17"/>
     </row>
@@ -6848,7 +6845,7 @@
         <v>1</v>
       </c>
       <c r="J147" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K147" s="17"/>
     </row>
@@ -6884,7 +6881,7 @@
         <v>0</v>
       </c>
       <c r="J148" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K148" s="17"/>
     </row>
@@ -6920,7 +6917,7 @@
         <v>0</v>
       </c>
       <c r="J149" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K149" s="17"/>
     </row>
@@ -6956,7 +6953,7 @@
         <v>0</v>
       </c>
       <c r="J150" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K150" s="17"/>
     </row>
@@ -6994,7 +6991,7 @@
       <c r="J151" s="17"/>
       <c r="K151" s="17"/>
     </row>
-    <row r="152" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
         <v>283</v>
       </c>
@@ -7027,7 +7024,7 @@
       </c>
       <c r="J152" s="17"/>
       <c r="K152" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="153" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
@@ -7062,7 +7059,7 @@
         <v>0</v>
       </c>
       <c r="J153" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K153" s="17"/>
     </row>
@@ -7098,7 +7095,7 @@
         <v>0</v>
       </c>
       <c r="J154" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K154" s="17"/>
     </row>
@@ -7134,11 +7131,11 @@
         <v>0</v>
       </c>
       <c r="J155" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K155" s="17"/>
     </row>
-    <row r="156" spans="2:11" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:11" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B156" s="3" t="s">
         <v>291</v>
       </c>
@@ -7171,10 +7168,10 @@
       </c>
       <c r="J156" s="17"/>
       <c r="K156" s="17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="157" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="157" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
         <v>293</v>
       </c>
@@ -7203,14 +7200,14 @@
         <v>Capítulo CID-10 da causa base do óbito</v>
       </c>
       <c r="I157" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J157" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K157" s="17"/>
     </row>
-    <row r="158" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B158" s="3" t="s">
         <v>295</v>
       </c>
@@ -7239,12 +7236,14 @@
         <v>Grupo CID-10 da causa base do óbito</v>
       </c>
       <c r="I158" s="7">
-        <v>0</v>
-      </c>
-      <c r="J158" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="J158" s="17" t="s">
+        <v>366</v>
+      </c>
       <c r="K158" s="17"/>
     </row>
-    <row r="159" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
         <v>297</v>
       </c>
@@ -7278,7 +7277,7 @@
       <c r="J159" s="17"/>
       <c r="K159" s="17"/>
     </row>
-    <row r="160" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B160" s="3" t="s">
         <v>299</v>
       </c>
@@ -7344,7 +7343,7 @@
         <v>0</v>
       </c>
       <c r="J161" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K161" s="17"/>
     </row>
@@ -7380,7 +7379,7 @@
         <v>0</v>
       </c>
       <c r="J162" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K162" s="17"/>
     </row>
@@ -7484,10 +7483,10 @@
         <v>1</v>
       </c>
       <c r="J165" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K165" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="166" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
@@ -8394,9 +8393,17 @@
     </row>
   </sheetData>
   <autoFilter ref="B3:K178">
-    <filterColumn colId="9">
+    <filterColumn colId="6">
       <filters>
-        <filter val="One hot"/>
+        <filter val="Capítulo CID-10 da causa base do óbito"/>
+        <filter val="Categoria CID-10 da causa base do óbito"/>
+        <filter val="Causa básica original, a primeira informação que entra nosistema"/>
+        <filter val="Causa básica, conforme a Classificação Internacional de Doença (CID), 10a. Revisão"/>
+        <filter val="Causa externa associada a uma causa materna"/>
+        <filter val="Causa selecionada sem re-seleção (novo SCB)"/>
+        <filter val="Grupo CID-10 da causa base do óbito"/>
+        <filter val="Subcategoria CID-10 da causa base do óbito"/>
+        <filter val="Versão do seletor de causa básica"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>